<commit_message>
changed authentifications method, added more apis
</commit_message>
<xml_diff>
--- a/uploads/users.xlsx
+++ b/uploads/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cirla\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B86BDB1-770F-471E-963A-CA499304B398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332F6C97-FB04-4E25-A28A-4DC6704DB3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4637" yWindow="4054" windowWidth="24686" windowHeight="13166" xr2:uid="{C7D265A7-CAB7-46D4-8388-D9FD25EFBA84}"/>
   </bookViews>
@@ -24,8 +24,142 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ancuta Cirlan</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{65B48217-DFD0-4C50-BD53-977560483335}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ancuta Cirlan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+poate fi doar "CD","SEC","ADM" sau "SG"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8A0F5218-8DD5-4A14-9C91-AB22E3221195}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ancuta Cirlan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+se completeaza doar pentru seful de grupa
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{33596973-7BC2-430A-B900-722B99A2914A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ancuta Cirlan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+se completeaza doar pentru seful de grupa
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DB6A1705-4D78-46CD-B477-CAA2B65B0516}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ancuta Cirlan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+se completeaza doar pentru seful de grupa
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{9811C7BE-6DB3-49E5-B5D1-98FF3C6D6917}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ancuta Cirlan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+se completeaza doar pentru cadrul didactic
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -73,13 +207,25 @@
   </si>
   <si>
     <t>ADM</t>
+  </si>
+  <si>
+    <t>maria bersa</t>
+  </si>
+  <si>
+    <t>maria@gmail.com</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>sic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +240,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -434,15 +593,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581A4D83-A5D0-45A5-9B7F-D985BF2B0AE1}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581A4D83-A5D0-45A5-9B7F-D985BF2B0AE1}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="22.3828125" customWidth="1"/>
     <col min="2" max="2" width="32.23046875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -520,12 +680,34 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>3114</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F67FC070-DF14-4638-9F86-3D46C16D1B11}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{21893504-89E5-4CA1-87F4-0B6A67928783}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{AF04DE86-BB6B-4B62-9BA4-391A70916D8E}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{25C4E25A-32E2-42C2-B5D3-A6D7C6B2D122}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>